<commit_message>
upload final data for han
</commit_message>
<xml_diff>
--- a/rnn/data/han/방사성/의암댐_2016.xlsx
+++ b/rnn/data/han/방사성/의암댐_2016.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotech/Desktop/NIA/water quality/test source/train_data/new/한강/방사성/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653AE61C-7B96-3B4A-97F9-8667A5111448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>year</t>
   </si>
@@ -122,6 +114,9 @@
   </si>
   <si>
     <t>iem_iod_131_dnsty_flag</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t>상반기</t>
@@ -151,31 +146,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -193,38 +180,23 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -233,10 +205,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -482,61 +454,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.71" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.57" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.71" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.57" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.43" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.71" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.43" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.71" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.71" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.29" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.43" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="24" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,18 +606,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
-      <c r="A2" s="5">
-        <v>42444.5</v>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -663,30 +629,30 @@
         <v>127.675555</v>
       </c>
       <c r="AA2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
-      <c r="A3" s="5">
-        <v>42628.5</v>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -698,20 +664,19 @@
         <v>127.675555</v>
       </c>
       <c r="AA3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD3">
         <v>1</v>
       </c>
     </row>
+    <row r="4"/>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>